<commit_message>
Aktualisierung der Projektnamen und der EffortEstimation
</commit_message>
<xml_diff>
--- a/Planning/EffortEstimation.xlsx
+++ b/Planning/EffortEstimation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabina\Documents\GitHub\NaoRemoteV\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabina\Documents\GitHub\NaoRemote\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Sabina</t>
   </si>
   <si>
-    <t>Taks</t>
-  </si>
-  <si>
     <t>Curr. Est</t>
   </si>
   <si>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>Hello World am Nao zum laufen bringen</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Tasks</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,8 +274,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -357,12 +378,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -430,21 +533,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -772,10 +894,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1138,10 +1260,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1367,7 +1489,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,164 +1503,241 @@
     <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="49" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="34">
         <v>42489</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="36">
         <v>42500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="D3" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="36" t="s">
+      <c r="G3" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="40">
+        <v>2</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="42">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="41">
+        <v>0</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="37">
+      <c r="B5" s="52">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="40">
+        <v>2</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="H4">
+      <c r="H6" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="s">
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="H5">
+      <c r="H7" s="54">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="37">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="H7">
-        <f>SUM(H4:H6)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43">
+        <f>SUM(H6:H7)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="33">
-        <v>2</v>
-      </c>
-      <c r="C9" s="33"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="43">
         <f>SUM(B4:B21)</f>
         <v>6</v>
       </c>
-      <c r="C22">
-        <f t="shared" ref="C22:E22" si="0">SUM(C4:C21)</f>
+      <c r="C22" s="43">
+        <f>SUM(C4:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="D22" s="42">
+        <f>SUM(D4:D21)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="43">
+        <f>SUM(E6:E21)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Android App File Transfer Beschreibung Excel aktualisiert
</commit_message>
<xml_diff>
--- a/Planning/EffortEstimation.xlsx
+++ b/Planning/EffortEstimation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>Sabina</t>
   </si>
   <si>
@@ -202,6 +199,12 @@
   </si>
   <si>
     <t>Herausfinden, wie ServerSocket am Nao funktioniert</t>
+  </si>
+  <si>
+    <t>Meli,Viki,Sabina</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -436,14 +439,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -452,13 +457,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -468,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,15 +552,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -570,6 +568,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -897,10 +903,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1263,10 +1269,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1489,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,60 +1506,57 @@
     <col min="1" max="1" width="71.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="57" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="54" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="32">
         <v>42489</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="48" t="s">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="55" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="34">
         <v>42500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="44" t="s">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>47</v>
       </c>
@@ -1563,23 +1566,22 @@
       <c r="C4" s="39">
         <v>0</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="39">
         <v>1.5</v>
       </c>
       <c r="E4" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="41">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="38">
         <v>1</v>
@@ -1587,126 +1589,163 @@
       <c r="C5" s="39">
         <v>0</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="39">
         <v>1</v>
       </c>
       <c r="E5" s="39">
         <v>0</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="41"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="F5" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="45">
+        <v>2</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0</v>
+      </c>
+      <c r="D6" s="46">
+        <v>2</v>
+      </c>
+      <c r="E6" s="46">
+        <v>0</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>55</v>
-      </c>
-      <c r="B6" s="50">
-        <v>2</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>56</v>
       </c>
       <c r="B7" s="38">
         <v>2</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="39">
+        <v>2</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52" t="s">
+      <c r="B8" s="45">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="45">
+        <v>1.5</v>
+      </c>
+      <c r="D8" s="46">
+        <v>0</v>
+      </c>
+      <c r="E8" s="46">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41">
-        <f>SUM(H7:H8)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="B9" s="38">
+        <v>3</v>
+      </c>
+      <c r="C9" s="39">
+        <v>3</v>
+      </c>
+      <c r="D9" s="39">
+        <v>0</v>
+      </c>
+      <c r="E9" s="39">
+        <v>3</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="52"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="45">
+        <v>1</v>
+      </c>
+      <c r="C10" s="45">
+        <v>0</v>
+      </c>
+      <c r="D10" s="46">
+        <v>1</v>
+      </c>
+      <c r="E10" s="46">
+        <v>0</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
       <c r="D16" s="35"/>
@@ -1743,27 +1782,27 @@
       <c r="E21" s="35"/>
     </row>
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41">
+      <c r="B23" s="40">
         <f>SUM(B4:B22)</f>
-        <v>7</v>
-      </c>
-      <c r="C23" s="41">
+        <v>12.5</v>
+      </c>
+      <c r="C23" s="40">
         <f>SUM(C4:C22)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="40">
+        <v>4.5</v>
+      </c>
+      <c r="D23" s="39">
         <f>SUM(D4:D22)</f>
-        <v>2.5</v>
-      </c>
-      <c r="E23" s="41">
+        <v>7.5</v>
+      </c>
+      <c r="E23" s="40">
         <f>SUM(E7:E22)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Server und Effort Estimation geändert
</commit_message>
<xml_diff>
--- a/Planning/EffortEstimation.xlsx
+++ b/Planning/EffortEstimation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -204,7 +204,7 @@
     <t>Meli,Viki,Sabina</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>Viki, Sabina</t>
   </si>
 </sst>
 </file>
@@ -562,12 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -576,6 +570,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -903,10 +903,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1269,10 +1269,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="12"/>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1506,7 @@
     <col min="1" max="1" width="71.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="52" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="32">
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="53" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="34">
@@ -1543,7 +1543,7 @@
       <c r="C3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="54" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="43" t="s">
@@ -1552,7 +1552,7 @@
       <c r="F3" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="51" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1564,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="39">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D4" s="39">
         <v>1.5</v>
@@ -1572,7 +1572,7 @@
       <c r="E4" s="39">
         <v>0</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="48" t="s">
         <v>56</v>
       </c>
       <c r="G4" s="40" t="s">
@@ -1587,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="39">
         <v>1</v>
@@ -1595,10 +1595,10 @@
       <c r="E5" s="39">
         <v>0</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="50" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="46">
         <v>2</v>
@@ -1618,7 +1618,7 @@
       <c r="E6" s="46">
         <v>0</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="49" t="s">
         <v>56</v>
       </c>
       <c r="G6" s="47" t="s">
@@ -1633,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="39">
         <v>2</v>
@@ -1641,10 +1641,10 @@
       <c r="E7" s="39">
         <v>0</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="50" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1656,19 +1656,19 @@
         <v>1.5</v>
       </c>
       <c r="C8" s="45">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D8" s="46">
+        <v>2</v>
+      </c>
+      <c r="E8" s="46">
         <v>0</v>
       </c>
-      <c r="E8" s="46">
-        <v>1.5</v>
-      </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="47" t="s">
         <v>60</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1679,18 +1679,20 @@
         <v>3</v>
       </c>
       <c r="C9" s="39">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" s="39">
+        <v>6</v>
+      </c>
+      <c r="E9" s="39">
         <v>0</v>
       </c>
-      <c r="E9" s="39">
-        <v>3</v>
-      </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="52"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
@@ -1700,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="46">
         <v>1</v>
@@ -1708,7 +1710,7 @@
       <c r="E10" s="46">
         <v>0</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="49" t="s">
         <v>56</v>
       </c>
       <c r="G10" s="47" t="s">
@@ -1794,15 +1796,15 @@
       </c>
       <c r="C23" s="40">
         <f>SUM(C4:C22)</f>
-        <v>4.5</v>
+        <v>15.5</v>
       </c>
       <c r="D23" s="39">
         <f>SUM(D4:D22)</f>
-        <v>7.5</v>
+        <v>15.5</v>
       </c>
       <c r="E23" s="40">
         <f>SUM(E7:E22)</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>